<commit_message>
Update schema + componenten
</commit_message>
<xml_diff>
--- a/componentenlijst elektronica.xlsx
+++ b/componentenlijst elektronica.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23231"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23530"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\kazim\Desktop\PEM\PEM_AutonomousCart\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{AE304CB7-ADCC-41E0-BB13-BE4428E2A4D3}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1872E890-41C3-4EC8-A0A4-C238CBFBF37F}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{BFFD4A00-7A2A-43CD-AE62-351A49A7BDFD}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5" uniqueCount="5">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7" uniqueCount="7">
   <si>
     <t>Klemblokken</t>
   </si>
@@ -49,6 +49,12 @@
   </si>
   <si>
     <t>item</t>
+  </si>
+  <si>
+    <t>3,5 mm powerjack</t>
+  </si>
+  <si>
+    <t>2,5 mm powerjack</t>
   </si>
 </sst>
 </file>
@@ -420,15 +426,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DA867641-A15C-4963-9A5A-C245B0EED393}">
-  <dimension ref="A1:C2"/>
+  <dimension ref="A1:C4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C11" sqref="C11"/>
+      <selection activeCell="C17" sqref="C17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="12.7109375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="17.28515625" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="255.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
@@ -452,6 +458,22 @@
       </c>
       <c r="C2" s="1" t="s">
         <v>1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A3">
+        <v>2</v>
+      </c>
+      <c r="B3" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A4">
+        <v>1</v>
+      </c>
+      <c r="B4" t="s">
+        <v>6</v>
       </c>
     </row>
   </sheetData>

</xml_diff>